<commit_message>
Strong releationships implemented and consent changes in excel
</commit_message>
<xml_diff>
--- a/Scealextric/DATA/Consent Request.xlsx
+++ b/Scealextric/DATA/Consent Request.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padraigmitchell/Google Drive/Fourth Year/Final Year Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padraigmitchell/git/EntertainMe/Scealextric/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,225 +27,225 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Conset Request</t>
   </si>
   <si>
-    <t>Would you like a story?</t>
-  </si>
-  <si>
-    <t>Want a story?</t>
-  </si>
-  <si>
-    <t>Fancy a story?</t>
-  </si>
-  <si>
-    <t>How about a story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Want me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Fancy a story told by me?</t>
-  </si>
-  <si>
-    <t>How about I tell you a story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tweet you a story?</t>
-  </si>
-  <si>
-    <t>Fancy a story in tweets?</t>
-  </si>
-  <si>
-    <t>Want a story in tweets?</t>
-  </si>
-  <si>
-    <t>How about I tweet you a story?</t>
-  </si>
-  <si>
-    <t>Would you like an entertaining story?</t>
-  </si>
-  <si>
-    <t>Want an entertaining story?</t>
-  </si>
-  <si>
-    <t>Fancy an entertaining story?</t>
-  </si>
-  <si>
-    <t>How about a entertaining story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Want me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Fancy an entertaining story told by me?</t>
-  </si>
-  <si>
-    <t>How about I tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tweet you an entertaing story</t>
-  </si>
-  <si>
-    <t>Want an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>How about I tweet you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Fancy an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy a story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about I tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tweet you story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot,  want a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about I tweet you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy an entertaining story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about I tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tweet you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about I tweet you an entertaining story? </t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about I tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tweet you story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin,  want a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about I tweet you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about I tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tweet you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about I tweet you an entertaining story? </t>
+    <t xml:space="preserve">Would you like a story about </t>
+  </si>
+  <si>
+    <t>a and b?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fancy a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How about a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you like me to tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want me to tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fancy a story told by me about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How about I tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you like me to tweet you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want a story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fancy a story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How about I tweet you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you like an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want an entertaining story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fancy an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fancy an entertaining story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you like me to tweet you an entertaing story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How about I tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fancy an entertaining story told by me about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want me to tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you like me to tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How about a entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How about I tweet you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, fancy a story told by me about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, would you like a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, want a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, fancy a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, would you like me to tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, want me to tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about I tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, would you like me to tweet you story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot,  want a story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, fancy a story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about I tweet you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, would you like an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, want an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, fancy an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, would you like me to tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, want me to tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, fancy an entertaining story told by me about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about I tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, would you like me to tweet you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, want an entertaining story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, fancy an entertaining story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about I tweet you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, would you like a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, want a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, want me to tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story told by me about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about I tell you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tweet you story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin,  want a story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about I tweet you a story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, would you like an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, want an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, want me to tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story told by me about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about I tell you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tweet you an entertaining story about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, want an entertaining story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story in tweets about </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about I tweet you an entertaining story about  </t>
   </si>
 </sst>
 </file>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A73"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B10"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,164 +581,167 @@
     <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -828,17 +831,17 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>